<commit_message>
Fixed incorrect package in SN74HCT245. Should have been TSSOP instead of SOIP.
</commit_message>
<xml_diff>
--- a/Hardware/bom/EncoderBoard_revB.xlsx
+++ b/Hardware/bom/EncoderBoard_revB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\Documents\Git\EosControl\Hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1013E7DF-C322-48EA-A2D4-D9CC53507941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6F4101-3A54-489B-B826-5578E22EB909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="5070" windowWidth="35145" windowHeight="16545" xr2:uid="{4FF78B83-AA82-492C-B8ED-FE0D2479E479}"/>
+    <workbookView xWindow="3180" yWindow="4395" windowWidth="32850" windowHeight="17445" xr2:uid="{4FF78B83-AA82-492C-B8ED-FE0D2479E479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>http://www.ti.com/lit/gpn/sn74HC245</t>
   </si>
   <si>
-    <t>SN74HCT245DWR</t>
-  </si>
-  <si>
     <t xml:space="preserve">U7 </t>
   </si>
   <si>
@@ -361,6 +358,9 @@
   </si>
   <si>
     <t>128x32_I2C_OLED_SSD1306</t>
+  </si>
+  <si>
+    <t>SN74HCT245PWR</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
   </cols>
@@ -1248,76 +1248,76 @@
         <v>81</v>
       </c>
       <c r="G22" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
         <v>93</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>94</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>95</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>96</v>
-      </c>
-      <c r="G23" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
         <v>99</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>100</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>101</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>102</v>
-      </c>
-      <c r="G24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
       <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
         <v>105</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>106</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>107</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>108</v>
-      </c>
-      <c r="G25" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>